<commit_message>
Added all files to git
</commit_message>
<xml_diff>
--- a/doc/DB Structure.xlsx
+++ b/doc/DB Structure.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="22">
   <si>
     <t>QuestionAnswer</t>
   </si>
@@ -60,9 +60,6 @@
     <t>Book</t>
   </si>
   <si>
-    <t>QuestionAnsType</t>
-  </si>
-  <si>
     <t>QuestionId</t>
   </si>
   <si>
@@ -75,19 +72,16 @@
     <t>SessionId</t>
   </si>
   <si>
-    <t>SectionSession</t>
-  </si>
-  <si>
     <t>SectionId</t>
   </si>
   <si>
-    <t>SectionBook</t>
-  </si>
-  <si>
     <t>BookId</t>
   </si>
   <si>
-    <t>SectionType</t>
+    <t>SectionQuestionType</t>
+  </si>
+  <si>
+    <t>QuestionAnswerSessionId</t>
   </si>
 </sst>
 </file>
@@ -426,24 +420,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J12"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -460,7 +454,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -477,7 +471,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -494,7 +488,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -502,7 +496,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -510,82 +504,56 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>1</v>
+      </c>
+      <c r="D10" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" t="s">
         <v>14</v>
       </c>
-      <c r="D9" t="s">
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" t="s">
         <v>17</v>
       </c>
-      <c r="F9" t="s">
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D14" t="s">
         <v>19</v>
-      </c>
-      <c r="H9" t="s">
-        <v>21</v>
-      </c>
-      <c r="J9" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>1</v>
-      </c>
-      <c r="D10" t="s">
-        <v>1</v>
-      </c>
-      <c r="F10" t="s">
-        <v>1</v>
-      </c>
-      <c r="H10" t="s">
-        <v>1</v>
-      </c>
-      <c r="J10" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>15</v>
-      </c>
-      <c r="D11" t="s">
-        <v>15</v>
-      </c>
-      <c r="F11" t="s">
-        <v>18</v>
-      </c>
-      <c r="H11" t="s">
-        <v>20</v>
-      </c>
-      <c r="J11" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>16</v>
-      </c>
-      <c r="D12" t="s">
-        <v>18</v>
-      </c>
-      <c r="F12" t="s">
-        <v>20</v>
-      </c>
-      <c r="H12" t="s">
-        <v>22</v>
-      </c>
-      <c r="J12" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Removed resharper files from github
</commit_message>
<xml_diff>
--- a/doc/DB Structure.xlsx
+++ b/doc/DB Structure.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="24">
   <si>
     <t>QuestionAnswer</t>
   </si>
@@ -82,6 +82,12 @@
   </si>
   <si>
     <t>QuestionAnswerSessionId</t>
+  </si>
+  <si>
+    <t>Answers</t>
+  </si>
+  <si>
+    <t>Option</t>
   </si>
 </sst>
 </file>
@@ -420,10 +426,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I14"/>
+  <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -437,7 +443,7 @@
     <col min="10" max="10" width="20.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -453,8 +459,11 @@
       <c r="I1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -470,8 +479,11 @@
       <c r="I2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -487,8 +499,11 @@
       <c r="I3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -496,7 +511,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -504,17 +519,17 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>20</v>
       </c>
@@ -522,7 +537,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>1</v>
       </c>
@@ -530,7 +545,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>21</v>
       </c>
@@ -538,7 +553,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>15</v>
       </c>
@@ -546,12 +561,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D13" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D14" t="s">
         <v>19</v>
       </c>

</xml_diff>